<commit_message>
Added My sprint tasks
</commit_message>
<xml_diff>
--- a/Gedcom_project.xlsx
+++ b/Gedcom_project.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swara\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\parth\OneDrive\Documents\Study_Docs\Agile_Methods\Group Project\CS555-WS3-TM02-2022FALL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFFCEB96-F6CA-4D21-A2A8-12A4D4C1302B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{972216C4-737A-4C8B-A883-FAF883D64C7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <sheet name="Sprint4" sheetId="7" r:id="rId8"/>
     <sheet name="Stories" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="218">
   <si>
     <t>Initials</t>
   </si>
@@ -627,9 +627,6 @@
     <t>SP</t>
   </si>
   <si>
-    <t>swarajsingpatil@gmail.conSwarajsingPatil</t>
-  </si>
-  <si>
     <t>SSS</t>
   </si>
   <si>
@@ -645,25 +642,58 @@
     <t>Swarajsing Anandsing</t>
   </si>
   <si>
-    <t>shoaibshah2400@gmail.com-</t>
+    <t>Swarajsing</t>
   </si>
   <si>
-    <r>
-      <t>Shoaib-byte</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <color theme="10"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
-      <t> </t>
-    </r>
+    <t>CS555-WS3-TM02-2022FALL</t>
   </si>
   <si>
-    <t>Swarajsing</t>
+    <t>Sangle</t>
+  </si>
+  <si>
+    <t>PJS</t>
+  </si>
+  <si>
+    <t>Pratik Jitendra</t>
+  </si>
+  <si>
+    <t>psangle@Stevens.edu</t>
+  </si>
+  <si>
+    <t>swarajsingpatil@gmail.com</t>
+  </si>
+  <si>
+    <t>SwarajsingPatil</t>
+  </si>
+  <si>
+    <t>shoaibshah2400@gmail.com</t>
+  </si>
+  <si>
+    <t>grindo26</t>
+  </si>
+  <si>
+    <t>RT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rucha </t>
+  </si>
+  <si>
+    <t>Tirodkar</t>
+  </si>
+  <si>
+    <t>Rucha1999</t>
+  </si>
+  <si>
+    <t>Pratik</t>
+  </si>
+  <si>
+    <t>Est Size(Lines)</t>
+  </si>
+  <si>
+    <t>Est Time(Minutes)</t>
+  </si>
+  <si>
+    <t>Shoaib-byte</t>
   </si>
 </sst>
 </file>
@@ -674,7 +704,7 @@
     <numFmt numFmtId="164" formatCode="m/d"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -710,13 +740,6 @@
       <sz val="10"/>
       <color theme="10"/>
       <name val="Verdana"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color theme="10"/>
-      <name val="Verdana"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -759,7 +782,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -786,7 +809,8 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -941,7 +965,7 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-JE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="261410492"/>
@@ -1005,7 +1029,7 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-JE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="751384951"/>
@@ -1143,7 +1167,7 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-JE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2018318546"/>
@@ -1207,7 +1231,7 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-JE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1881607879"/>
@@ -2051,16 +2075,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.36328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.81640625" customWidth="1"/>
-    <col min="2" max="2" width="6.36328125" customWidth="1"/>
+    <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.36328125" customWidth="1"/>
-    <col min="4" max="5" width="20.36328125" customWidth="1"/>
+    <col min="4" max="4" width="34.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.36328125" customWidth="1"/>
     <col min="6" max="26" width="10.6328125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2107,45 +2132,66 @@
         <v>194</v>
       </c>
       <c r="B2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>195</v>
+        <v>206</v>
+      </c>
+      <c r="E2" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>198</v>
-      </c>
       <c r="D3" s="15" t="s">
-        <v>201</v>
-      </c>
-      <c r="E3" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="4" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
+      <c r="D4" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="5" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
+      <c r="A5" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>212</v>
+      </c>
       <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>213</v>
+      </c>
     </row>
     <row r="6" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="7" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2154,7 +2200,9 @@
       <c r="D9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="2"/>
+      <c r="E9" s="2" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="10" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="11" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3151,7 +3199,7 @@
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{19FE6E2D-4958-4143-BC20-95C55EBFF258}"/>
     <hyperlink ref="D3" r:id="rId2" xr:uid="{BE58D3F2-3A6C-421A-904F-28BE0D0F4C03}"/>
-    <hyperlink ref="E3" r:id="rId3" tooltip="View all commits by Shoaib-byte" display="https://github.com/grindo26/CS555-WS3-TM02-2022FALL/commits?author=Shoaib-byte" xr:uid="{5248C7F0-6F3C-48D1-86D6-1F087701599F}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{0E7338DE-1241-4B1F-8F5A-86C57E2C2722}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
@@ -3163,7 +3211,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:C6"/>
+      <selection activeCell="B7" sqref="B7:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.36328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -12708,21 +12756,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="156" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView zoomScale="156" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.36328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.6328125" customWidth="1"/>
-    <col min="2" max="2" width="62.453125" customWidth="1"/>
-    <col min="3" max="3" width="10.36328125" customWidth="1"/>
-    <col min="4" max="4" width="10.6328125" customWidth="1"/>
-    <col min="5" max="5" width="9.81640625" customWidth="1"/>
-    <col min="6" max="6" width="14" customWidth="1"/>
-    <col min="7" max="7" width="9" customWidth="1"/>
-    <col min="8" max="8" width="12.6328125" customWidth="1"/>
-    <col min="9" max="9" width="10.81640625" customWidth="1"/>
+    <col min="1" max="1" width="8.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.08984375" bestFit="1" customWidth="1"/>
     <col min="10" max="26" width="10.6328125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -12740,10 +12788,10 @@
         <v>10</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>34</v>
+        <v>215</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>35</v>
+        <v>216</v>
       </c>
       <c r="G1" s="12" t="s">
         <v>36</v>
@@ -12807,7 +12855,7 @@
         <v>160</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>193</v>
@@ -12828,7 +12876,7 @@
         <v>166</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>193</v>
@@ -12842,13 +12890,45 @@
       <c r="I5" s="4"/>
     </row>
     <row r="6" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="2"/>
+      <c r="A6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" t="s">
+        <v>167</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="E6">
+        <v>120</v>
+      </c>
+      <c r="F6">
+        <v>600</v>
+      </c>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="3"/>
+    <row r="7" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" t="s">
+        <v>168</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="E7">
+        <v>50</v>
+      </c>
+      <c r="F7">
+        <v>200</v>
+      </c>
       <c r="I7" s="4"/>
     </row>
     <row r="8" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>